<commit_message>
manto 7.6 até antes de outliers
</commit_message>
<xml_diff>
--- a/doc/ACAP manto PH 7.3 08-04-21.xlsx
+++ b/doc/ACAP manto PH 7.3 08-04-21.xlsx
@@ -513,11 +513,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85248256"/>
-        <c:axId val="102940672"/>
+        <c:axId val="141789056"/>
+        <c:axId val="141790592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85248256"/>
+        <c:axId val="141789056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102940672"/>
+        <c:crossAx val="141790592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102940672"/>
+        <c:axId val="141790592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85248256"/>
+        <c:crossAx val="141789056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7929,7 +7929,7 @@
   <dimension ref="A1:I1249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30900,7 +30900,7 @@
   <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>